<commit_message>
wip narrative excel files
</commit_message>
<xml_diff>
--- a/src/assets/narrative/branch_a.xlsx
+++ b/src/assets/narrative/branch_a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schne\GitHub\run-it-again\src\assets\narrative\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F04FC5A-22BB-428A-8267-D09AFEF0265B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C23E59-AD69-4396-A4C8-A847E515278D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{C6B0DF71-00FB-4C6D-B239-677EC6E0ABF1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Initial reveal</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Reporting perimeter entry, currently breaching main entranceat the objective.</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>Quit smiling, private! Get those eyes on the horizon before I turn you into a fucking stain on the wall!</t>
   </si>
   <si>
@@ -105,13 +102,82 @@
   </si>
   <si>
     <t>Gunfire and static</t>
+  </si>
+  <si>
+    <t>Sputterings of remaining gun fire.</t>
+  </si>
+  <si>
+    <t>Man down! Call for evac! Call for -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Break. We have sustained casualities but will continue as planned. </t>
+  </si>
+  <si>
+    <t>NEXT BRANCH</t>
+  </si>
+  <si>
+    <t>Copy that, we are Oscar Mike. Alpha out.</t>
+  </si>
+  <si>
+    <t>Command, this is Alpha. Report sustained contact with 5 targets to our rear.</t>
+  </si>
+  <si>
+    <t>Copy that, command. We'll see it through. Alpha out.</t>
+  </si>
+  <si>
+    <t>NEXT BRANCH + Determined</t>
+  </si>
+  <si>
+    <t>NEXT BRANCH + Retreat</t>
+  </si>
+  <si>
+    <t>ETA 2 minutes to objective. May lose radio contact underground.  Alpha out.</t>
+  </si>
+  <si>
+    <t>1: Retreat</t>
+  </si>
+  <si>
+    <t>2: Silence</t>
+  </si>
+  <si>
+    <t>3: Pressure</t>
+  </si>
+  <si>
+    <t>2nd timer</t>
+  </si>
+  <si>
+    <t>2nd timer Retreat</t>
+  </si>
+  <si>
+    <t>Command, this is Alpha. Requesting immediate backup - entrance cannot be reached. Repeat!</t>
+  </si>
+  <si>
+    <t>Entrance cannot-- *pained shout*</t>
+  </si>
+  <si>
+    <t>Don't you fucking let go of that trigger! Don't you fucking let go!</t>
+  </si>
+  <si>
+    <t>Static.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">But best I can tell, they didn't bring climbing gear. </t>
+  </si>
+  <si>
+    <t>Calling for backup --- entrance ---- clogged. Evac path --- further support.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Command, this is Alpha. Reporting no resistance ---- level. Break.</t>
+  </si>
+  <si>
+    <t>Setting--- breach ----, Alpha out.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +187,14 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -148,13 +222,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4952649-252D-4D6F-9D1C-B601BF72B0B0}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,26 +562,44 @@
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="F1" s="3">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3">
+        <v>3</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -515,11 +610,37 @@
         <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -527,12 +648,38 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="4" spans="1:19" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -542,10 +689,32 @@
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -553,12 +722,32 @@
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -566,79 +755,193 @@
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+    </row>
+    <row r="7" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>